<commit_message>
Changed from py2 to py3
</commit_message>
<xml_diff>
--- a/SysArch.xlsx
+++ b/SysArch.xlsx
@@ -34,16 +34,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="56">
   <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>BrakeSensor</t>
+  </si>
+  <si>
     <t>BlockType</t>
   </si>
   <si>
     <t>SEN</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>BrakeSensor</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>2YpdEY8oORx3fjk5kcs5-1</t>
   </si>
   <si>
     <t>Parent</t>
@@ -52,18 +58,12 @@
     <t>CHASSIS</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>2YpdEY8oORx3fjk5kcs5-1</t>
+    <t>BSPD</t>
   </si>
   <si>
     <t>ECU</t>
   </si>
   <si>
-    <t>BSPD</t>
-  </si>
-  <si>
     <t>2YpdEY8oORx3fjk5kcs5-2</t>
   </si>
   <si>
@@ -106,46 +106,67 @@
     <t>Sa5RoMOKzB4C418BSFVM-2</t>
   </si>
   <si>
+    <t>BrakePressure</t>
+  </si>
+  <si>
+    <t>DIG</t>
+  </si>
+  <si>
     <t>Source</t>
   </si>
   <si>
-    <t>DIG</t>
-  </si>
-  <si>
-    <t>BrakePressure</t>
-  </si>
-  <si>
     <t>Target</t>
   </si>
   <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;%Name% : %BlockType%&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>UnderSeat</t>
+  </si>
+  <si>
+    <t>InputVoltage</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>MaxCurrent</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
     <t>placeholders</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;%Name% : %BlockType%&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>MaxCurrent</t>
-  </si>
-  <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>UnderSeat</t>
-  </si>
-  <si>
-    <t>InputVoltage</t>
-  </si>
-  <si>
-    <t>24</t>
+    <t>&lt;span style="white-space: normal"&gt;&lt;b&gt;%Name% : %BlockType%&lt;/b&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>PedalAssembly</t>
+  </si>
+  <si>
+    <t>MfgPartNumber</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>OutputType</t>
+  </si>
+  <si>
+    <t>Digital</t>
+  </si>
+  <si>
+    <t>OutputMin</t>
   </si>
   <si>
     <t>OutputMax</t>
@@ -157,33 +178,18 @@
     <t>OutputParameter</t>
   </si>
   <si>
-    <t>OutputMin</t>
-  </si>
-  <si>
-    <t>OutputType</t>
-  </si>
-  <si>
-    <t>Digital</t>
-  </si>
-  <si>
-    <t>&lt;span style="white-space: normal"&gt;&lt;b&gt;%Name% : %BlockType%&lt;/b&gt;&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>MfgPartNumber</t>
-  </si>
-  <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>PedalAssembly</t>
-  </si>
-  <si>
     <t>System</t>
   </si>
   <si>
     <t>BrakeSystem</t>
   </si>
   <si>
+    <t>VoltageHigh</t>
+  </si>
+  <si>
+    <t>VoltageLow</t>
+  </si>
+  <si>
     <t>Protocol</t>
   </si>
   <si>
@@ -191,12 +197,6 @@
   </si>
   <si>
     <t>2YpdEY8oORx3fjk5kcs5-3</t>
-  </si>
-  <si>
-    <t>VoltageHigh</t>
-  </si>
-  <si>
-    <t>VoltageLow</t>
   </si>
   <si>
     <t>Sa5RoMOKzB4C418BSFVM-3</t>
@@ -573,24 +573,24 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -601,24 +601,24 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -629,38 +629,38 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -671,38 +671,38 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -723,22 +723,22 @@
         <v>28</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -746,22 +746,22 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -769,22 +769,22 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -826,80 +826,80 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G1" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" t="s">
         <v>55</v>
-      </c>
-      <c r="E3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -989,13 +989,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
         <v>27</v>
@@ -1003,13 +1003,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
@@ -1030,13 +1030,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
         <v>27</v>
@@ -1044,16 +1044,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1074,10 +1074,10 @@
         <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>30</v>
@@ -1086,16 +1086,16 @@
         <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1103,10 +1103,10 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
@@ -1115,16 +1115,16 @@
         <v>33</v>
       </c>
       <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1135,7 +1135,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
@@ -1144,16 +1144,16 @@
         <v>33</v>
       </c>
       <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
         <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1171,135 +1171,135 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
         <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" t="s">
-        <v>30</v>
-      </c>
       <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
         <v>45</v>
       </c>
-      <c r="J1" t="s">
-        <v>32</v>
-      </c>
       <c r="K1" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="L1" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="M1" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="N1" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
         <v>43</v>
       </c>
-      <c r="H3" t="s">
-        <v>44</v>
-      </c>
       <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
         <v>46</v>
       </c>
-      <c r="J3" t="s">
-        <v>33</v>
-      </c>
       <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" t="s">
         <v>15</v>
       </c>
-      <c r="L3" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
-        <v>37</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>